<commit_message>
Update code 2 11/11/2021
</commit_message>
<xml_diff>
--- a/Databases/HoaHoc.xlsx
+++ b/Databases/HoaHoc.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
-  <si>
-    <t>Clo hóa</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
   <si>
     <t xml:space="preserve">clo hóa PVC thu đc tơ clorin và khí HCL, tơ clorin dùng để làm thảm. HCl có thể tẩy gỉ sắt thép, trung hòa PH,.. thậm chí có thể tiếp tục tạo ra PVC </t>
   </si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>Chưng khô ( 450-800 C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dechlorinate </t>
   </si>
 </sst>
 </file>
@@ -413,9 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -426,10 +424,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C1">
         <v>4</v>
@@ -437,10 +435,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -448,10 +446,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -459,10 +457,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -470,10 +468,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -481,10 +479,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -492,10 +490,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -503,10 +501,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -520,10 +518,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>2</v>

</xml_diff>